<commit_message>
super/fix: modifed excel template file
</commit_message>
<xml_diff>
--- a/public/Leads.xlsx
+++ b/public/Leads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Upwork\Orr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9834F6BD-B78C-4DF9-9CFC-43AFBA5502D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835624CD-B01A-4468-B2AD-FF63063A1EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{11793BAE-D751-4E64-B148-E19772FE18B3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
   <si>
     <t>Sylvan Kunde V</t>
   </si>
@@ -280,6 +280,21 @@
   </si>
   <si>
     <t>Origin</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>vip</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -631,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891A6732-A77C-45DA-8589-835EDA3330FD}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +660,7 @@
     <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -658,8 +673,11 @@
       <c r="D1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -672,8 +690,11 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -686,8 +707,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -701,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -714,8 +738,11 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -728,8 +755,11 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -743,7 +773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -756,8 +786,11 @@
       <c r="D8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -770,8 +803,11 @@
       <c r="D9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -784,8 +820,11 @@
       <c r="D10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -798,8 +837,11 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -813,7 +855,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -826,8 +868,11 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -840,8 +885,11 @@
       <c r="D14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -854,8 +902,11 @@
       <c r="D15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -869,7 +920,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -882,8 +933,11 @@
       <c r="D17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -896,8 +950,11 @@
       <c r="D18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -910,8 +967,11 @@
       <c r="D19" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -924,8 +984,11 @@
       <c r="D20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -938,8 +1001,11 @@
       <c r="D21" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>

</xml_diff>